<commit_message>
major fixes and restructuring
</commit_message>
<xml_diff>
--- a/anthropos/static/files/all_individs.xlsx
+++ b/anthropos/static/files/all_individs.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,55 +540,55 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Гермонасса-2111-212</t>
+          <t>Аржан-543-2020-2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Гермонасса</t>
+          <t>Аржан-543</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>п.212</t>
+          <t>п.2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ранний железный век, Античное время, Эпоха переселения народов</t>
+          <t>Поздний бронзовый век, Ранний железный век</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ильина Т.А.</t>
+          <t>Поляков А.В.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Южный федеральный округ</t>
+          <t>Сибирский федеральный округ</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Краснодарский край</t>
+          <t>Респ Тыва</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>36.713953</t>
+          <t>23.000000</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>45.218670</t>
+          <t>45.000000</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>2111</v>
+        <v>2020</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>15-16</t>
+          <t>2-6</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -598,34 +598,34 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>женский</t>
+          <t>не определен</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>средняя</t>
+          <t>плохая</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>sfassaasfa</t>
+          <t>ЛОЫАРЛОЫ ПАЛОЫЛОЛЫА ыфвфвфыв</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R2" s="2" t="n">
-        <v>45129.61915362279</v>
+        <v>45119.38295040985</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T2" s="2" t="n">
-        <v>45129.61915458663</v>
+        <v>45135.71290080703</v>
       </c>
     </row>
     <row r="3">
@@ -634,7 +634,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Великий новгород-1999-2</t>
+          <t>Великий новгород-1342-2131</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>к.1/п.2</t>
+          <t>п.2131</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>1999</v>
+        <v>1342</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -692,34 +692,34 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>мужской</t>
+          <t>не определен</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>плохая</t>
+          <t>удовлетворительная</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>afasfsafasfassfa</t>
+          <t>another random comment</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R3" s="2" t="n">
-        <v>45134.46050734502</v>
+        <v>45118.68942703947</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T3" s="2" t="n">
-        <v>45134.46050741447</v>
+        <v>45134.87599239686</v>
       </c>
     </row>
     <row r="4">
@@ -801,19 +801,19 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R4" s="2" t="n">
-        <v>45134.46127481342</v>
+        <v>45134.46050734502</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T4" s="2" t="n">
-        <v>45134.46127486779</v>
+        <v>45134.46050741447</v>
       </c>
     </row>
     <row r="5">
@@ -822,92 +822,92 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Гермонасса-2012-2</t>
+          <t>Великий новгород-1999-2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Гермонасса</t>
+          <t>Великий новгород</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>к.12/п.2</t>
+          <t>к.1/п.2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Ранний железный век, Античное время, Эпоха переселения народов</t>
+          <t>Развитое средневековье</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Ильина Т.А.</t>
+          <t>Гайдуков П.Г.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Южный федеральный округ</t>
+          <t>Северо-Западный федеральный округ</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Краснодарский край</t>
+          <t>Новгородская обл</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>36.713953</t>
+          <t>14.000000</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>45.218670</t>
+          <t>15.000000</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>2012</v>
+        <v>1999</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>22-35</t>
+          <t>20-30</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>кремация</t>
+          <t>ингумация</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>женский</t>
+          <t>мужской</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>хорошая</t>
+          <t>плохая</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Посткраниальный скелет</t>
+          <t>afasfsafasfassfa</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R5" s="2" t="n">
-        <v>45117.41454492303</v>
+        <v>45134.46127481342</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T5" s="2" t="n">
-        <v>45118.46982249552</v>
+        <v>45134.46127486779</v>
       </c>
     </row>
     <row r="6">
@@ -916,92 +916,92 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Минино ii-2002-41</t>
+          <t>Волна-11-2010-2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Минино ii</t>
+          <t>Волна-11</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>п.41</t>
+          <t>к.1/п.2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Раннее средневековье, Развитое средневековье</t>
+          <t>Ранний железный век, Античное время</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Макаров Н.А.</t>
+          <t>Монахов С.Ю.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Северо-Западный федеральный округ</t>
+          <t>Южный федеральный округ</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Вологодская обл</t>
+          <t>Краснодарский край</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>12.000000</t>
+          <t>18.000000</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>15.000000</t>
+          <t>19.000000</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>2002</v>
+        <v>2010</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>27-37</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>ингумация</t>
+          <t>кремация</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>не определен</t>
+          <t>мужской</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>удовлетворительная</t>
+          <t>плохая</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Череп разрушен, отдельные кости посткраниального скелета. отдельные кости мелкие в пакетах 41-43</t>
+          <t>ну просто так чтоб было что то продолжаем проверим фыаврфгафгурагшурпфш щш йщцшкйцшг йфывфыаафыавыайфафыафыафафыафыафыафафы йгцшкгйцшгк йзкг зшйцгк йзшцгкйцзшг кйцзшгк йзцщ</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R6" s="2" t="n">
-        <v>45118.48118956037</v>
+        <v>45119.38251706091</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T6" s="2" t="n">
-        <v>45118.48119167701</v>
+        <v>45134.88917448132</v>
       </c>
     </row>
     <row r="7">
@@ -1010,92 +1010,92 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Минино ii-2002-42</t>
+          <t>Гермонасса-2012-2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Минино ii</t>
+          <t>Гермонасса</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>п.42</t>
+          <t>к.12/п.2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Раннее средневековье, Развитое средневековье</t>
+          <t>Ранний железный век, Античное время, Эпоха переселения народов</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Макаров Н.А.</t>
+          <t>Ильина Т.А.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Северо-Западный федеральный округ</t>
+          <t>Южный федеральный округ</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Вологодская обл</t>
+          <t>Краснодарский край</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>12.000000</t>
+          <t>36.713953</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>15.000000</t>
+          <t>45.218670</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>2002</v>
+        <v>2012</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>6-7</t>
+          <t>22-35</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>ингумация</t>
+          <t>кремация</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>не определен</t>
+          <t>женский</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>удовлетворительная</t>
+          <t>хорошая</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>отдельные кости посткраниального скелета, 19 зубов, череп разрушен</t>
+          <t>Посткраниальный скелет</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R7" s="2" t="n">
-        <v>45118.48920740103</v>
+        <v>45117.41454492303</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T7" s="2" t="n">
-        <v>45118.48921092833</v>
+        <v>45118.46982249552</v>
       </c>
     </row>
     <row r="8">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R8" s="2" t="n">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T8" s="2" t="n">
@@ -1198,55 +1198,55 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Великий новгород-1342-2131</t>
+          <t>Гермонасса-2111-212</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Великий новгород</t>
+          <t>Гермонасса</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>п.2131</t>
+          <t>п.212</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Развитое средневековье</t>
+          <t>Ранний железный век, Античное время, Эпоха переселения народов</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Гайдуков П.Г.</t>
+          <t>Ильина Т.А.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Северо-Западный федеральный округ</t>
+          <t>Южный федеральный округ</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Новгородская обл</t>
+          <t>Краснодарский край</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>14.000000</t>
+          <t>36.713953</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>15.000000</t>
+          <t>45.218670</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>1342</v>
+        <v>2111</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>20-30</t>
+          <t>15-16</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1256,34 +1256,34 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>не определен</t>
+          <t>женский</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>удовлетворительная</t>
+          <t>средняя</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>another random comment</t>
+          <t>sfassaasfa</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R9" s="2" t="n">
-        <v>45118.68942703947</v>
+        <v>45129.61915362279</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T9" s="2" t="n">
-        <v>45118.6894305989</v>
+        <v>45129.61915458663</v>
       </c>
     </row>
     <row r="10">
@@ -1292,22 +1292,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Суздаль-1999-1-2</t>
+          <t>Минино ii-2002-41</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Суздаль</t>
+          <t>Минино ii</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>к.1/п.2</t>
+          <t>п.41</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Энеолит</t>
+          <t>Раннее средневековье, Развитое средневековье</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1317,12 +1317,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Дальневосточный федеральный округ</t>
+          <t>Северо-Западный федеральный округ</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Магаданская обл</t>
+          <t>Вологодская обл</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1332,15 +1332,15 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>13.000000</t>
+          <t>15.000000</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>1999</v>
+        <v>2002</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>25-30</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1350,34 +1350,34 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>мужской</t>
+          <t>не определен</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>хорошая</t>
+          <t>удовлетворительная</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Тупо рандомный коммент</t>
+          <t>Череп разрушен, отдельные кости посткраниального скелета. отдельные кости мелкие в пакетах 41-43</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R10" s="2" t="n">
-        <v>45119.37980261447</v>
+        <v>45118.48118956037</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T10" s="2" t="n">
-        <v>45119.37980372266</v>
+        <v>45118.48119167701</v>
       </c>
     </row>
     <row r="11">
@@ -1386,22 +1386,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Шекшово-1765-2</t>
+          <t>Минино ii-2002-42</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Шекшово</t>
+          <t>Минино ii</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>к.1/п.2</t>
+          <t>п.42</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Палеолит</t>
+          <t>Раннее средневековье, Развитое средневековье</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1411,12 +1411,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Центральный федеральный округ</t>
+          <t>Северо-Западный федеральный округ</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Ивановская обл</t>
+          <t>Вологодская обл</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1426,52 +1426,52 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>13.000000</t>
+          <t>15.000000</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>1765</v>
+        <v>2002</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>45-49</t>
+          <t>6-7</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>кремация</t>
+          <t>ингумация</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>женский</t>
+          <t>не определен</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>плохая</t>
+          <t>удовлетворительная</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Опять рандомный коммент КЕКЛУЛ</t>
+          <t>отдельные кости посткраниального скелета, 19 зубов, череп разрушен</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R11" s="2" t="n">
-        <v>45119.38027628961</v>
+        <v>45118.48920740103</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T11" s="2" t="n">
-        <v>45119.38028059875</v>
+        <v>45118.48921092833</v>
       </c>
     </row>
     <row r="12">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R12" s="2" t="n">
@@ -1561,11 +1561,11 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T12" s="2" t="n">
-        <v>45119.38097371529</v>
+        <v>45134.87346390077</v>
       </c>
     </row>
     <row r="13">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R13" s="2" t="n">
@@ -1655,7 +1655,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T13" s="2" t="n">
@@ -1668,12 +1668,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Волна-11-2010-2</t>
+          <t>Суздаль-1999-1-2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Волна-11</t>
+          <t>Суздаль</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1683,45 +1683,45 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ранний железный век, Античное время</t>
+          <t>Энеолит</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Монахов С.Ю.</t>
+          <t>Макаров Н.А.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Южный федеральный округ</t>
+          <t>Дальневосточный федеральный округ</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Краснодарский край</t>
+          <t>Магаданская обл</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>18.000000</t>
+          <t>12.000000</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>19.000000</t>
+          <t>13.000000</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>2010</v>
+        <v>1999</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>27-37</t>
+          <t>25-30</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>кремация</t>
+          <t>ингумация</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1731,29 +1731,29 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>плохая</t>
+          <t>хорошая</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>ну просто так чтоб было что то</t>
+          <t>Тупо рандомный коммент</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R14" s="2" t="n">
-        <v>45119.38251706091</v>
+        <v>45119.37980261447</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T14" s="2" t="n">
-        <v>45119.38251797527</v>
+        <v>45119.37980372266</v>
       </c>
     </row>
     <row r="15">
@@ -1762,88 +1762,92 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Мухкай-1231-1-2</t>
+          <t>Улан-iv-2000-25-2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Мухкай</t>
+          <t>Улан-iv</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>к.1/п.2</t>
+          <t>к.25/п.2</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Палеолит</t>
+          <t>Средний бронзовый век</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Амирханов Х.А.</t>
+          <t>Шишлина Н.И.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Северо-Кавказский федеральный округ</t>
+          <t>Южный федеральный округ</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Респ Дагестан</t>
+          <t>Ростовская обл</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>16.000000</t>
+          <t>44.100000</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>29.000000</t>
+          <t>55.200000</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>1231</v>
-      </c>
-      <c r="L15" t="inlineStr"/>
+        <v>2000</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>50-60</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>кремация</t>
+          <t>ингумация</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>мужской</t>
+          <t>женский</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>плохая</t>
+          <t>хорошая</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>eqweqwewqq</t>
+          <t>mbglghffxgfxfcv,</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R15" s="2" t="n">
-        <v>45134.60619459991</v>
+        <v>45128.59741799543</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T15" s="2" t="n">
-        <v>45134.60619465463</v>
+        <v>45128.59741892288</v>
       </c>
     </row>
     <row r="16">
@@ -1852,65 +1856,65 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Аржан-543-2020-2</t>
+          <t>Улан-iv-2004-1-2</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Аржан-543</t>
+          <t>Улан-iv</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>п.2</t>
+          <t>к.1/п.2</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Поздний бронзовый век, Ранний железный век</t>
+          <t>Средний бронзовый век</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Поляков А.В.</t>
+          <t>Шишлина Н.И.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Сибирский федеральный округ</t>
+          <t>Южный федеральный округ</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Респ Тыва</t>
+          <t>Ростовская обл</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>23.000000</t>
+          <t>44.100000</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>45.000000</t>
+          <t>55.200000</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>2020</v>
+        <v>2004</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2-6</t>
+          <t>15-25</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>кремация</t>
+          <t>ингумация</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>не определен</t>
+          <t>мужской</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1920,24 +1924,24 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>ЛОЫАРЛОЫПАЛОЫЛОЛЫАыфвфвфыв</t>
+          <t>fsafasfafasfas</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R16" s="2" t="n">
-        <v>45119.38295040985</v>
+        <v>45128.59629810395</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T16" s="2" t="n">
-        <v>45121.65898648987</v>
+        <v>45128.61556644237</v>
       </c>
     </row>
     <row r="17">
@@ -1946,7 +1950,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Улан-iv-2000-25-2</t>
+          <t>Улан-iv-2010-1-2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1956,7 +1960,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>к.25/п.2</t>
+          <t>к.1/п.2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1990,48 +1994,48 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>50-60</t>
+          <t>25+</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>ингумация</t>
+          <t>кремация</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>женский</t>
+          <t>мужской</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>хорошая</t>
+          <t>плохая</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>mbglghffxgfxfcv,</t>
+          <t>asfsffa</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R17" s="2" t="n">
-        <v>45128.59741799543</v>
+        <v>45134.62308453361</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T17" s="2" t="n">
-        <v>45128.59741892288</v>
+        <v>45134.62308458463</v>
       </c>
     </row>
     <row r="18">
@@ -2040,12 +2044,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Рэндом памятник-2000-1-2</t>
+          <t>Шекшово-1765-2</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Рэндом памятник</t>
+          <t>Шекшово</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2060,17 +2064,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Окладников А.П.</t>
+          <t>Макаров Н.А.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Сибирский федеральный округ</t>
+          <t>Центральный федеральный округ</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Респ Алтай</t>
+          <t>Ивановская обл</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2084,12 +2088,16 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>2000</v>
-      </c>
-      <c r="L18" t="inlineStr"/>
+        <v>1765</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>45-49</t>
+        </is>
+      </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>ингумация</t>
+          <t>кремация</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -2099,311 +2107,29 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>хорошая</t>
+          <t>плохая</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>fasfass</t>
+          <t>Опять рандомный коммент КЕКЛУЛ</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="R18" s="2" t="n">
-        <v>45134.60730020816</v>
+        <v>45119.38027628961</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Strokov A.</t>
+          <t>Строков А.А.</t>
         </is>
       </c>
       <c r="T18" s="2" t="n">
-        <v>45134.60730026302</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Улан-iv-2010-1-2</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Улан-iv</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>к.1/п.2</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Средний бронзовый век</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Шишлина Н.И.</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Южный федеральный округ</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Ростовская обл</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>44.100000</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>55.200000</t>
-        </is>
-      </c>
-      <c r="K19" t="n">
-        <v>2010</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>25+</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>кремация</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>мужской</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>плохая</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>asfsffa</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>Strokov A.</t>
-        </is>
-      </c>
-      <c r="R19" s="2" t="n">
-        <v>45134.62308453361</v>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>Strokov A.</t>
-        </is>
-      </c>
-      <c r="T19" s="2" t="n">
-        <v>45134.62308458463</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Улан-iv-2004-1-2</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Улан-iv</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>к.1/п.2</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Средний бронзовый век</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Шишлина Н.И.</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Южный федеральный округ</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Ростовская обл</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>44.100000</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>55.200000</t>
-        </is>
-      </c>
-      <c r="K20" t="n">
-        <v>2004</v>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>15-25</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>ингумация</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>мужской</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>плохая</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>fsafasfafasfas</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>Strokov A.</t>
-        </is>
-      </c>
-      <c r="R20" s="2" t="n">
-        <v>45128.59629810395</v>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>Strokov A.</t>
-        </is>
-      </c>
-      <c r="T20" s="2" t="n">
-        <v>45128.61556644237</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Волна-11-2007-12-56</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Волна-11</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>к.12/п.56</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Ранний железный век, Античное время</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Монахов С.Ю.</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Южный федеральный округ</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Краснодарский край</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>18.000000</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>19.000000</t>
-        </is>
-      </c>
-      <c r="K21" t="n">
-        <v>2007</v>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>10-20</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>ингумация</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>мужской</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>средняя</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>safdasfasfasf</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>Strokov A.</t>
-        </is>
-      </c>
-      <c r="R21" s="2" t="n">
-        <v>45129.61806789311</v>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>Strokov A.</t>
-        </is>
-      </c>
-      <c r="T21" s="2" t="n">
-        <v>45129.61806882593</v>
+        <v>45119.38028059875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>